<commit_message>
Updated names and add kettle
</commit_message>
<xml_diff>
--- a/ILRG_ORAM_P_parcels/ILRG_ORAM_P_parcels-media/ILRG_ORAM_P_parcels.xlsx
+++ b/ILRG_ORAM_P_parcels/ILRG_ORAM_P_parcels-media/ILRG_ORAM_P_parcels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\ILRG\oram\ODK Forms\ILRG_ORAM_odk_forms\ILRG_ORAM_P_parcels\ILRG_ORAM_P_parcels-media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA7C442-ED88-4326-9DE9-96D7F680DCA1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26354DE2-BED6-402A-843E-03CA166CD000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3338" uniqueCount="1589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3338" uniqueCount="1588">
   <si>
     <t>type</t>
   </si>
@@ -4025,9 +4025,6 @@
   </si>
   <si>
     <t>other_name</t>
-  </si>
-  <si>
-    <t>Qual é a outra nome da pessoa, se tiver?</t>
   </si>
   <si>
     <t>mother_name</t>
@@ -4824,9 +4821,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="41" x14ac:knownFonts="1">
+  <fonts count="42" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -5136,491 +5140,492 @@
   </borders>
   <cellStyleXfs count="240">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="233" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="235" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="233" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="235" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="235" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="235" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="235" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="235" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="0" xfId="239" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="239" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="239" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="239" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="239" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="239"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="2"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="239" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="239" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="239" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="239" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="239" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="239"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="240">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -6201,11 +6206,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q142"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C146" sqref="C146"/>
+      <selection pane="bottomRight" activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6268,7 +6273,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="30" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="N1" s="26" t="s">
         <v>11</v>
@@ -6333,7 +6338,7 @@
         <v>1181</v>
       </c>
       <c r="O6" s="93" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="7" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -6361,7 +6366,7 @@
         <v>1148</v>
       </c>
       <c r="C9" s="112" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="10" spans="1:17" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -6372,7 +6377,7 @@
         <v>30</v>
       </c>
       <c r="C10" s="83" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="J10" s="49" t="s">
         <v>22</v>
@@ -6607,7 +6612,7 @@
         <v>1263</v>
       </c>
       <c r="G23" s="102" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="J23" s="49" t="s">
         <v>22</v>
@@ -6704,7 +6709,7 @@
         <v>1266</v>
       </c>
       <c r="C29" s="92" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="E29" s="32"/>
       <c r="F29" s="32"/>
@@ -6723,7 +6728,7 @@
         <v>1265</v>
       </c>
       <c r="C30" s="75" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="G30" s="49" t="s">
         <v>1268</v>
@@ -6778,10 +6783,10 @@
         <v>67</v>
       </c>
       <c r="B33" s="89" t="s">
+        <v>1452</v>
+      </c>
+      <c r="C33" s="92" t="s">
         <v>1453</v>
-      </c>
-      <c r="C33" s="92" t="s">
-        <v>1454</v>
       </c>
       <c r="E33" s="32"/>
       <c r="F33" s="32"/>
@@ -6884,7 +6889,7 @@
         <v>29</v>
       </c>
       <c r="B40" s="73" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="C40" s="49" t="s">
         <v>1311</v>
@@ -6907,7 +6912,7 @@
         <v>1126</v>
       </c>
       <c r="E41" s="49" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="42" spans="1:12" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -6949,10 +6954,10 @@
         <v>1158</v>
       </c>
       <c r="C44" s="86" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="G44" s="81" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="J44" s="50" t="s">
         <v>22</v>
@@ -6960,16 +6965,16 @@
     </row>
     <row r="45" spans="1:12" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="94" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="B45" s="89" t="s">
+        <v>1526</v>
+      </c>
+      <c r="C45" s="86" t="s">
         <v>1527</v>
       </c>
-      <c r="C45" s="86" t="s">
-        <v>1528</v>
-      </c>
       <c r="G45" s="81" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="J45" s="92" t="s">
         <v>22</v>
@@ -6988,7 +6993,7 @@
         <v>1320</v>
       </c>
       <c r="C47" s="113" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="J47" s="34" t="s">
         <v>22</v>
@@ -7019,7 +7024,7 @@
         <v>77</v>
       </c>
       <c r="B49" s="78" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="C49" s="79" t="s">
         <v>1319</v>
@@ -7033,7 +7038,7 @@
         <v>93</v>
       </c>
       <c r="B50" s="67" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>1325</v>
@@ -7078,7 +7083,7 @@
         <v>1328</v>
       </c>
       <c r="C53" s="108" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="54" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -7086,10 +7091,10 @@
         <v>26</v>
       </c>
       <c r="B54" s="65" t="s">
+        <v>1329</v>
+      </c>
+      <c r="C54" s="49" t="s">
         <v>1330</v>
-      </c>
-      <c r="C54" s="49" t="s">
-        <v>1331</v>
       </c>
       <c r="J54" s="49" t="s">
         <v>22</v>
@@ -7100,10 +7105,10 @@
         <v>26</v>
       </c>
       <c r="B55" s="65" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C55" s="49" t="s">
         <v>1332</v>
-      </c>
-      <c r="C55" s="49" t="s">
-        <v>1333</v>
       </c>
       <c r="J55" s="49" t="s">
         <v>22</v>
@@ -7120,10 +7125,10 @@
         <v>93</v>
       </c>
       <c r="B57" s="67" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="L57" s="49" t="s">
         <v>95</v>
@@ -7134,10 +7139,10 @@
         <v>98</v>
       </c>
       <c r="B58" s="65" t="s">
+        <v>1334</v>
+      </c>
+      <c r="C58" s="49" t="s">
         <v>1335</v>
-      </c>
-      <c r="C58" s="49" t="s">
-        <v>1336</v>
       </c>
       <c r="J58" s="49" t="s">
         <v>22</v>
@@ -7169,7 +7174,7 @@
         <v>26</v>
       </c>
       <c r="B60" s="73" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="C60" s="50" t="s">
         <v>1130</v>
@@ -7192,7 +7197,7 @@
         <v>67</v>
       </c>
       <c r="B62" s="65" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="C62" s="49" t="s">
         <v>1153</v>
@@ -7209,16 +7214,16 @@
         <v>17</v>
       </c>
       <c r="B63" s="65" t="s">
+        <v>1338</v>
+      </c>
+      <c r="C63" s="49" t="s">
         <v>1339</v>
       </c>
-      <c r="C63" s="49" t="s">
+      <c r="G63" s="49" t="s">
         <v>1340</v>
       </c>
-      <c r="G63" s="49" t="s">
+      <c r="H63" s="49" t="s">
         <v>1341</v>
-      </c>
-      <c r="H63" s="49" t="s">
-        <v>1342</v>
       </c>
       <c r="J63" s="49" t="s">
         <v>22</v>
@@ -7232,13 +7237,13 @@
         <v>1131</v>
       </c>
       <c r="B64" s="65" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="C64" s="49" t="s">
         <v>1132</v>
       </c>
       <c r="G64" s="49" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="J64" s="49" t="s">
         <v>22</v>
@@ -7252,10 +7257,10 @@
         <v>63</v>
       </c>
       <c r="B65" s="65" t="s">
+        <v>1344</v>
+      </c>
+      <c r="N65" s="49" t="s">
         <v>1345</v>
-      </c>
-      <c r="N65" s="49" t="s">
-        <v>1346</v>
       </c>
     </row>
     <row r="66" spans="1:15" s="49" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7263,13 +7268,13 @@
         <v>31</v>
       </c>
       <c r="B66" s="65" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="C66" s="104" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="G66" s="84" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="67" spans="1:15" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -7277,13 +7282,13 @@
         <v>1314</v>
       </c>
       <c r="B67" s="95" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="C67" s="86" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="G67" s="50" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="J67" s="50" t="s">
         <v>22</v>
@@ -7291,16 +7296,16 @@
     </row>
     <row r="68" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="92" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="B68" s="95" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="C68" s="86" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="G68" s="81" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="J68" s="92" t="s">
         <v>22</v>
@@ -7311,7 +7316,7 @@
         <v>93</v>
       </c>
       <c r="B69" s="67" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>1133</v>
@@ -7325,10 +7330,10 @@
         <v>122</v>
       </c>
       <c r="B70" s="65" t="s">
+        <v>1347</v>
+      </c>
+      <c r="C70" s="49" t="s">
         <v>1348</v>
-      </c>
-      <c r="C70" s="49" t="s">
-        <v>1349</v>
       </c>
       <c r="J70" s="49" t="s">
         <v>22</v>
@@ -7342,10 +7347,10 @@
         <v>26</v>
       </c>
       <c r="B71" s="65" t="s">
+        <v>1349</v>
+      </c>
+      <c r="C71" s="49" t="s">
         <v>1350</v>
-      </c>
-      <c r="C71" s="49" t="s">
-        <v>1351</v>
       </c>
       <c r="H71" s="49" t="s">
         <v>123</v>
@@ -7359,10 +7364,10 @@
         <v>26</v>
       </c>
       <c r="B72" s="65" t="s">
+        <v>1351</v>
+      </c>
+      <c r="C72" s="49" t="s">
         <v>1352</v>
-      </c>
-      <c r="C72" s="49" t="s">
-        <v>1353</v>
       </c>
       <c r="H72" s="49" t="s">
         <v>1152</v>
@@ -7376,13 +7381,13 @@
         <v>17</v>
       </c>
       <c r="B73" s="65" t="s">
+        <v>1353</v>
+      </c>
+      <c r="C73" s="49" t="s">
         <v>1354</v>
       </c>
-      <c r="C73" s="49" t="s">
-        <v>1355</v>
-      </c>
       <c r="H73" s="83" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="L73" s="49" t="s">
         <v>28</v>
@@ -7393,13 +7398,13 @@
         <v>17</v>
       </c>
       <c r="B74" s="65" t="s">
+        <v>1355</v>
+      </c>
+      <c r="C74" s="49" t="s">
         <v>1356</v>
       </c>
-      <c r="C74" s="49" t="s">
-        <v>1357</v>
-      </c>
       <c r="H74" s="83" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="L74" s="49" t="s">
         <v>28</v>
@@ -7410,10 +7415,10 @@
         <v>67</v>
       </c>
       <c r="B75" s="65" t="s">
+        <v>1357</v>
+      </c>
+      <c r="C75" s="49" t="s">
         <v>1358</v>
-      </c>
-      <c r="C75" s="49" t="s">
-        <v>1359</v>
       </c>
     </row>
     <row r="76" spans="1:15" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -7427,10 +7432,10 @@
         <v>67</v>
       </c>
       <c r="B77" s="65" t="s">
+        <v>1359</v>
+      </c>
+      <c r="C77" s="49" t="s">
         <v>1360</v>
-      </c>
-      <c r="C77" s="49" t="s">
-        <v>1361</v>
       </c>
     </row>
     <row r="78" spans="1:15" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -7441,10 +7446,10 @@
         <v>120</v>
       </c>
       <c r="C78" s="49" t="s">
+        <v>1361</v>
+      </c>
+      <c r="G78" s="49" t="s">
         <v>1362</v>
-      </c>
-      <c r="G78" s="49" t="s">
-        <v>1363</v>
       </c>
       <c r="H78" s="49" t="s">
         <v>1154</v>
@@ -7458,13 +7463,13 @@
         <v>31</v>
       </c>
       <c r="B79" s="65" t="s">
+        <v>1363</v>
+      </c>
+      <c r="C79" s="103" t="s">
+        <v>1579</v>
+      </c>
+      <c r="O79" s="49" t="s">
         <v>1364</v>
-      </c>
-      <c r="C79" s="103" t="s">
-        <v>1580</v>
-      </c>
-      <c r="O79" s="49" t="s">
-        <v>1365</v>
       </c>
     </row>
     <row r="80" spans="1:15" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -7472,7 +7477,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="65" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="C80" s="50" t="s">
         <v>1134</v>
@@ -7481,7 +7486,7 @@
         <v>22</v>
       </c>
       <c r="M80" s="80" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="81" spans="1:15" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -7501,7 +7506,7 @@
         <v>80</v>
       </c>
       <c r="M81" s="80" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="82" spans="1:15" s="49" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -7509,13 +7514,13 @@
         <v>31</v>
       </c>
       <c r="B82" s="65" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C82" s="69" t="s">
+        <v>1382</v>
+      </c>
+      <c r="O82" s="49" t="s">
         <v>1368</v>
-      </c>
-      <c r="C82" s="69" t="s">
-        <v>1383</v>
-      </c>
-      <c r="O82" s="49" t="s">
-        <v>1369</v>
       </c>
     </row>
     <row r="83" spans="1:15" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -7523,16 +7528,16 @@
         <v>79</v>
       </c>
       <c r="B83" s="65" t="s">
+        <v>1369</v>
+      </c>
+      <c r="C83" s="76" t="s">
         <v>1370</v>
-      </c>
-      <c r="C83" s="76" t="s">
-        <v>1371</v>
       </c>
       <c r="J83" s="49" t="s">
         <v>22</v>
       </c>
       <c r="M83" s="80" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="84" spans="1:15" s="49" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -7540,13 +7545,13 @@
         <v>79</v>
       </c>
       <c r="B84" s="65" t="s">
+        <v>1371</v>
+      </c>
+      <c r="C84" s="76" t="s">
         <v>1372</v>
       </c>
-      <c r="C84" s="76" t="s">
-        <v>1373</v>
-      </c>
       <c r="M84" s="80" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="85" spans="1:15" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -7554,10 +7559,10 @@
         <v>26</v>
       </c>
       <c r="B85" s="65" t="s">
+        <v>1373</v>
+      </c>
+      <c r="C85" s="49" t="s">
         <v>1374</v>
-      </c>
-      <c r="C85" s="49" t="s">
-        <v>1375</v>
       </c>
       <c r="H85" s="49" t="s">
         <v>1154</v>
@@ -7574,16 +7579,16 @@
         <v>26</v>
       </c>
       <c r="B86" s="65" t="s">
+        <v>1375</v>
+      </c>
+      <c r="C86" s="49" t="s">
         <v>1376</v>
       </c>
-      <c r="C86" s="49" t="s">
+      <c r="H86" s="49" t="s">
         <v>1377</v>
       </c>
-      <c r="H86" s="49" t="s">
+      <c r="I86" s="50" t="s">
         <v>1378</v>
-      </c>
-      <c r="I86" s="50" t="s">
-        <v>1379</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
@@ -7596,10 +7601,10 @@
         <v>29</v>
       </c>
       <c r="B88" s="82" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="C88" s="81" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="H88" s="81" t="s">
         <v>129</v>
@@ -7616,13 +7621,13 @@
         <v>77</v>
       </c>
       <c r="B89" s="74" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="E89" s="49" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="90" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -7630,10 +7635,10 @@
         <v>26</v>
       </c>
       <c r="B90" s="95" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="C90" s="50" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="J90" s="32" t="s">
         <v>22</v>
@@ -7644,30 +7649,30 @@
         <v>1315</v>
       </c>
       <c r="B91" s="73" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="C91" s="76" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="J91" s="32" t="s">
         <v>22</v>
       </c>
       <c r="L91" s="97" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" s="49" t="s">
+        <v>1433</v>
+      </c>
+      <c r="B92" s="65" t="s">
         <v>1434</v>
-      </c>
-      <c r="B92" s="65" t="s">
-        <v>1435</v>
       </c>
       <c r="C92" s="34" t="s">
         <v>128</v>
       </c>
       <c r="G92" s="111" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="H92" s="32"/>
       <c r="J92" s="34" t="s">
@@ -7687,10 +7692,10 @@
         <v>67</v>
       </c>
       <c r="B94" s="65" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="C94" s="113" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="F94" s="49"/>
       <c r="J94" s="34" t="s">
@@ -7702,13 +7707,13 @@
         <v>29</v>
       </c>
       <c r="B95" s="73" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="C95" s="49" t="s">
         <v>1323</v>
       </c>
       <c r="G95" s="49" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="H95" s="34" t="s">
         <v>62</v>
@@ -7722,13 +7727,13 @@
         <v>77</v>
       </c>
       <c r="B96" s="78" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="C96" s="79" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="E96" s="80" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="97" spans="1:14" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -7736,7 +7741,7 @@
         <v>93</v>
       </c>
       <c r="B97" s="67" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>1325</v>
@@ -7750,7 +7755,7 @@
         <v>26</v>
       </c>
       <c r="B98" s="96" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="C98" s="49" t="s">
         <v>96</v>
@@ -7764,7 +7769,7 @@
         <v>26</v>
       </c>
       <c r="B99" s="96" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="C99" s="49" t="s">
         <v>97</v>
@@ -7778,10 +7783,10 @@
         <v>26</v>
       </c>
       <c r="B100" s="96" t="s">
-        <v>1564</v>
-      </c>
-      <c r="C100" s="49" t="s">
-        <v>1329</v>
+        <v>1563</v>
+      </c>
+      <c r="C100" s="114" t="s">
+        <v>1583</v>
       </c>
     </row>
     <row r="101" spans="1:14" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -7789,10 +7794,10 @@
         <v>26</v>
       </c>
       <c r="B101" s="96" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="C101" s="49" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="J101" s="49" t="s">
         <v>22</v>
@@ -7803,10 +7808,10 @@
         <v>26</v>
       </c>
       <c r="B102" s="96" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="C102" s="49" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="J102" s="49" t="s">
         <v>22</v>
@@ -7823,10 +7828,10 @@
         <v>93</v>
       </c>
       <c r="B104" s="67" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="L104" s="49" t="s">
         <v>95</v>
@@ -7837,10 +7842,10 @@
         <v>98</v>
       </c>
       <c r="B105" s="96" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="C105" s="49" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="J105" s="49" t="s">
         <v>22</v>
@@ -7854,7 +7859,7 @@
         <v>99</v>
       </c>
       <c r="B106" s="95" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="C106" s="50" t="s">
         <v>100</v>
@@ -7872,7 +7877,7 @@
         <v>26</v>
       </c>
       <c r="B107" s="95" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="C107" s="50" t="s">
         <v>1130</v>
@@ -7895,7 +7900,7 @@
         <v>67</v>
       </c>
       <c r="B109" s="96" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="C109" s="49" t="s">
         <v>1153</v>
@@ -7912,16 +7917,16 @@
         <v>17</v>
       </c>
       <c r="B110" s="96" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="C110" s="49" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="G110" s="98" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="H110" s="49" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="J110" s="49" t="s">
         <v>22</v>
@@ -7935,13 +7940,13 @@
         <v>1131</v>
       </c>
       <c r="B111" s="96" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="C111" s="49" t="s">
         <v>1132</v>
       </c>
       <c r="G111" s="98" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="J111" s="49" t="s">
         <v>22</v>
@@ -7955,10 +7960,10 @@
         <v>63</v>
       </c>
       <c r="B112" s="96" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="N112" s="98" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="113" spans="1:15" s="49" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7966,13 +7971,13 @@
         <v>31</v>
       </c>
       <c r="B113" s="96" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="C113" s="99" t="s">
+        <v>1573</v>
+      </c>
+      <c r="G113" s="97" t="s">
         <v>1574</v>
-      </c>
-      <c r="G113" s="97" t="s">
-        <v>1575</v>
       </c>
     </row>
     <row r="114" spans="1:15" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -7980,7 +7985,7 @@
         <v>93</v>
       </c>
       <c r="B114" s="67" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>1133</v>
@@ -7994,10 +7999,10 @@
         <v>122</v>
       </c>
       <c r="B115" s="96" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="C115" s="49" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="J115" s="49" t="s">
         <v>22</v>
@@ -8011,10 +8016,10 @@
         <v>26</v>
       </c>
       <c r="B116" s="96" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="C116" s="49" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="H116" s="49" t="s">
         <v>123</v>
@@ -8028,10 +8033,10 @@
         <v>26</v>
       </c>
       <c r="B117" s="96" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="C117" s="49" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="H117" s="49" t="s">
         <v>1152</v>
@@ -8045,10 +8050,10 @@
         <v>17</v>
       </c>
       <c r="B118" s="96" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="C118" s="49" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="L118" s="49" t="s">
         <v>28</v>
@@ -8059,10 +8064,10 @@
         <v>17</v>
       </c>
       <c r="B119" s="96" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="C119" s="49" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="L119" s="49" t="s">
         <v>28</v>
@@ -8073,10 +8078,10 @@
         <v>67</v>
       </c>
       <c r="B120" s="96" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="C120" s="49" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="121" spans="1:15" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -8090,10 +8095,10 @@
         <v>67</v>
       </c>
       <c r="B122" s="96" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="C122" s="49" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="123" spans="1:15" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -8101,13 +8106,13 @@
         <v>26</v>
       </c>
       <c r="B123" s="96" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="C123" s="49" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="G123" s="98" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="H123" s="49" t="s">
         <v>1154</v>
@@ -8121,13 +8126,13 @@
         <v>31</v>
       </c>
       <c r="B124" s="96" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="C124" s="103" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="O124" s="49" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="125" spans="1:15" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -8135,7 +8140,7 @@
         <v>79</v>
       </c>
       <c r="B125" s="96" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="C125" s="50" t="s">
         <v>1134</v>
@@ -8144,7 +8149,7 @@
         <v>22</v>
       </c>
       <c r="M125" s="80" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="126" spans="1:15" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -8152,7 +8157,7 @@
         <v>79</v>
       </c>
       <c r="B126" s="96" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="C126" s="49" t="s">
         <v>1135</v>
@@ -8164,7 +8169,7 @@
         <v>80</v>
       </c>
       <c r="M126" s="80" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="127" spans="1:15" s="49" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -8172,13 +8177,13 @@
         <v>31</v>
       </c>
       <c r="B127" s="96" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="C127" s="69" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="O127" s="49" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="128" spans="1:15" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -8186,16 +8191,16 @@
         <v>79</v>
       </c>
       <c r="B128" s="96" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="C128" s="76" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="J128" s="49" t="s">
         <v>22</v>
       </c>
       <c r="M128" s="80" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="129" spans="1:14" s="49" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -8203,13 +8208,13 @@
         <v>79</v>
       </c>
       <c r="B129" s="96" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="C129" s="76" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="M129" s="80" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="130" spans="1:14" s="49" customFormat="1" x14ac:dyDescent="0.25">
@@ -8217,10 +8222,10 @@
         <v>26</v>
       </c>
       <c r="B130" s="96" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="C130" s="49" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="H130" s="49" t="s">
         <v>1154</v>
@@ -8237,24 +8242,24 @@
         <v>26</v>
       </c>
       <c r="B131" s="96" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="C131" s="49" t="s">
+        <v>1376</v>
+      </c>
+      <c r="H131" s="49" t="s">
         <v>1377</v>
       </c>
-      <c r="H131" s="49" t="s">
+      <c r="I131" s="50" t="s">
         <v>1378</v>
-      </c>
-      <c r="I131" s="50" t="s">
-        <v>1379</v>
       </c>
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A132" s="49" t="s">
+        <v>1433</v>
+      </c>
+      <c r="B132" s="65" t="s">
         <v>1434</v>
-      </c>
-      <c r="B132" s="65" t="s">
-        <v>1435</v>
       </c>
       <c r="C132" s="34" t="s">
         <v>128</v>
@@ -8280,7 +8285,7 @@
         <v>87</v>
       </c>
       <c r="C134" s="92" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="D134" s="32"/>
       <c r="F134" s="32"/>
@@ -8295,7 +8300,7 @@
         <v>67</v>
       </c>
       <c r="B135" s="107" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="C135" s="34" t="s">
         <v>131</v>
@@ -8315,7 +8320,7 @@
         <v>88</v>
       </c>
       <c r="G136" s="106" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.25">
@@ -8346,7 +8351,7 @@
         <v>92</v>
       </c>
       <c r="N138" s="88" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.25">
@@ -8371,7 +8376,7 @@
         <v>79</v>
       </c>
       <c r="B141" s="89" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="C141" s="32" t="s">
         <v>1124</v>
@@ -9092,21 +9097,21 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="90" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B63" s="91" t="s">
+        <v>1448</v>
+      </c>
+      <c r="C63" s="90" t="s">
         <v>1447</v>
-      </c>
-      <c r="B63" s="91" t="s">
-        <v>1449</v>
-      </c>
-      <c r="C63" s="90" t="s">
-        <v>1448</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="90" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="B64" s="91" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>60</v>
@@ -9203,7 +9208,7 @@
         <v>1285</v>
       </c>
       <c r="B75" s="91" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>82</v>
@@ -9214,7 +9219,7 @@
         <v>1285</v>
       </c>
       <c r="B76" s="91" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>83</v>
@@ -9225,10 +9230,10 @@
         <v>1285</v>
       </c>
       <c r="B77" s="91" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="C77" s="90" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -9250,7 +9255,7 @@
         <v>112</v>
       </c>
       <c r="B80" s="91" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="C80" s="90" t="s">
         <v>113</v>
@@ -9261,7 +9266,7 @@
         <v>112</v>
       </c>
       <c r="B81" s="91" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="C81" s="90" t="s">
         <v>114</v>
@@ -9272,7 +9277,7 @@
         <v>112</v>
       </c>
       <c r="B82" s="91" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="C82" s="90" t="s">
         <v>115</v>
@@ -9283,7 +9288,7 @@
         <v>112</v>
       </c>
       <c r="B83" s="91" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="C83" s="90" t="s">
         <v>116</v>
@@ -9294,10 +9299,10 @@
         <v>112</v>
       </c>
       <c r="B84" s="91" t="s">
+        <v>1398</v>
+      </c>
+      <c r="C84" s="90" t="s">
         <v>1399</v>
-      </c>
-      <c r="C84" s="90" t="s">
-        <v>1400</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -9305,10 +9310,10 @@
         <v>112</v>
       </c>
       <c r="B85" s="91" t="s">
+        <v>1400</v>
+      </c>
+      <c r="C85" s="90" t="s">
         <v>1401</v>
-      </c>
-      <c r="C85" s="90" t="s">
-        <v>1402</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -9316,7 +9321,7 @@
         <v>112</v>
       </c>
       <c r="B86" s="91" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="C86" s="90" t="s">
         <v>117</v>
@@ -9327,7 +9332,7 @@
         <v>112</v>
       </c>
       <c r="B87" s="91" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="C87" s="90" t="s">
         <v>118</v>
@@ -9338,7 +9343,7 @@
         <v>112</v>
       </c>
       <c r="B88" s="91" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="C88" s="90" t="s">
         <v>119</v>
@@ -9371,10 +9376,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="58" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="B92" s="85" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="C92" s="9" t="s">
         <v>125</v>
@@ -9382,21 +9387,21 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="58" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="B93" s="85" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="C93" s="105" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="58" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="B94" s="85" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="C94" s="9" t="s">
         <v>126</v>
@@ -9404,10 +9409,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="58" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="B95" s="85" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="C95" s="9" t="s">
         <v>127</v>
@@ -9608,7 +9613,7 @@
         <v>101</v>
       </c>
       <c r="B116" s="70" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="C116" s="58" t="s">
         <v>102</v>
@@ -9621,7 +9626,7 @@
         <v>101</v>
       </c>
       <c r="B117" s="70" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="C117" s="58" t="s">
         <v>103</v>
@@ -9641,10 +9646,10 @@
         <v>105</v>
       </c>
       <c r="B119" s="70" t="s">
+        <v>1383</v>
+      </c>
+      <c r="C119" s="58" t="s">
         <v>1384</v>
-      </c>
-      <c r="C119" s="58" t="s">
-        <v>1385</v>
       </c>
       <c r="E119" s="71"/>
       <c r="F119" s="72"/>
@@ -9654,10 +9659,10 @@
         <v>105</v>
       </c>
       <c r="B120" s="70" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C120" s="58" t="s">
         <v>1386</v>
-      </c>
-      <c r="C120" s="58" t="s">
-        <v>1387</v>
       </c>
       <c r="E120" s="71"/>
       <c r="F120" s="72"/>
@@ -9667,10 +9672,10 @@
         <v>105</v>
       </c>
       <c r="B121" s="70" t="s">
+        <v>1387</v>
+      </c>
+      <c r="C121" s="58" t="s">
         <v>1388</v>
-      </c>
-      <c r="C121" s="58" t="s">
-        <v>1389</v>
       </c>
       <c r="E121" s="71"/>
       <c r="F121" s="72"/>
@@ -9680,10 +9685,10 @@
         <v>105</v>
       </c>
       <c r="B122" s="70" t="s">
+        <v>1389</v>
+      </c>
+      <c r="C122" s="58" t="s">
         <v>1390</v>
-      </c>
-      <c r="C122" s="58" t="s">
-        <v>1391</v>
       </c>
       <c r="E122" s="71"/>
       <c r="F122" s="72"/>
@@ -9698,7 +9703,7 @@
         <v>106</v>
       </c>
       <c r="B124" s="70" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="C124" s="58" t="s">
         <v>107</v>
@@ -9711,7 +9716,7 @@
         <v>106</v>
       </c>
       <c r="B125" s="70" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="C125" s="58" t="s">
         <v>108</v>
@@ -9724,7 +9729,7 @@
         <v>106</v>
       </c>
       <c r="B126" s="70" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="C126" s="58" t="s">
         <v>109</v>
@@ -9737,7 +9742,7 @@
         <v>106</v>
       </c>
       <c r="B127" s="70" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="C127" s="58" t="s">
         <v>110</v>
@@ -9750,7 +9755,7 @@
         <v>106</v>
       </c>
       <c r="B128" s="70" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="C128" s="58" t="s">
         <v>111</v>
@@ -9777,7 +9782,7 @@
         <v>1158</v>
       </c>
       <c r="B131" s="91" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="C131" s="43" t="s">
         <v>1160</v>
@@ -9788,10 +9793,10 @@
         <v>1158</v>
       </c>
       <c r="B132" s="91" t="s">
+        <v>1458</v>
+      </c>
+      <c r="C132" s="90" t="s">
         <v>1459</v>
-      </c>
-      <c r="C132" s="90" t="s">
-        <v>1460</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
@@ -9799,10 +9804,10 @@
     </row>
     <row r="134" spans="1:6" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="58" t="s">
+        <v>1410</v>
+      </c>
+      <c r="B134" s="70" t="s">
         <v>1411</v>
-      </c>
-      <c r="B134" s="70" t="s">
-        <v>1412</v>
       </c>
       <c r="C134" s="58" t="s">
         <v>1129</v>
@@ -9812,13 +9817,13 @@
     </row>
     <row r="135" spans="1:6" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="58" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="B135" s="70" t="s">
         <v>1245</v>
       </c>
       <c r="C135" s="58" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="E135" s="71"/>
       <c r="F135" s="72"/>
@@ -9828,370 +9833,370 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B137" s="91" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B138" s="91" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="C138" s="90" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B139" s="91" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="C139" s="43" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B140" s="91" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B141" s="91" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="C141" s="90" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B142" s="91" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B143" s="91" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="C143" s="90" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B144" s="91" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B145" s="91" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B146" s="91" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B147" s="91" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B148" s="91" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="C148" s="90" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B149" s="91" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B150" s="91" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="C150" s="90" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B151" s="91" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="C151" s="90" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B152" s="91" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="C152" s="90" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B153" s="91" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="C153" s="90" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B154" s="91" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="C154" s="90" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B155" s="91" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="C155" s="90" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B156" s="91" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B157" s="91" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C157" s="90" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B158" s="91" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="C158" s="90" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B159" s="91" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="C159" s="90" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B160" s="91" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B161" s="91" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B162" s="91" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="C162" s="90" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B163" s="91" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="C163" s="90" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B164" s="91" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="C164" s="90" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B165" s="91" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="C165" s="90" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B166" s="91" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="C166" s="90" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B167" s="91" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="C167" s="90" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B168" s="91" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="C168" s="90" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B169" s="91" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="C169" s="90" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B170" s="91" t="s">
         <v>1245</v>
@@ -35513,8 +35518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35548,10 +35553,10 @@
         <v>1172</v>
       </c>
       <c r="C2" s="45">
-        <v>201905093</v>
+        <v>201905094</v>
       </c>
       <c r="D2" s="101" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>